<commit_message>
Additional cleanup of unnecessary files
Some empty files were removed, and not-used files have been corrected, probably will be deleted in the near future
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SuppXLS/Scen_UC_Growth.xlsx
+++ b/TIMES-NZ/SuppXLS/Scen_UC_Growth.xlsx
@@ -1,32 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\veda\VEDA_Models\NZ_TIMES_model-v34_hydro\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\TIMES-NZ-Model-Files\TIMES-NZ\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEEDAE6-5241-4F93-A018-15767F11F9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_Growth" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Suleimenov Bakytzhan</author>
     <author>Amit Kanudia</author>
   </authors>
   <commentList>
-    <comment ref="G9" authorId="0" shapeId="0">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="1" shapeId="0">
+    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>~UC_T</t>
   </si>
@@ -154,12 +168,15 @@
   </si>
   <si>
     <t>T_P_B*ELC*</t>
+  </si>
+  <si>
+    <t>UC_T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -282,24 +299,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -310,9 +326,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="3"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -344,7 +360,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Right Brace 1"/>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -399,7 +421,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -446,7 +474,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -482,9 +516,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -522,9 +556,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -559,7 +593,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -594,7 +628,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -767,101 +801,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -880,59 +906,59 @@
       <c r="K9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>1</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="8">
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="N9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="M18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -943,75 +969,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C6:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="K7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="3:14" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1048,7 @@
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <f>721/10^6</f>
         <v>7.2099999999999996E-4</v>
       </c>

</xml_diff>